<commit_message>
added to doc folder AND added to Sharepoint added also Textfile with Sharepoint Links
git-svn-id: https://by-stsvn.bayer-ag.com/svn/DOC41WEBUI@890 7fa4df38-a670-11e2-8034-c9adf4be1a24
</commit_message>
<xml_diff>
--- a/trunk/DOC41WEBUI/docs/BDS DocTypes.xlsx
+++ b/trunk/DOC41WEBUI/docs/BDS DocTypes.xlsx
@@ -427,7 +427,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -446,12 +446,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -465,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -473,7 +467,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -778,7 +771,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.296875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1542,11 +1535,27 @@
       <c r="A31" s="2" t="s">
         <v>122</v>
       </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="4" t="s">
         <v>123</v>
       </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">

</xml_diff>